<commit_message>
TeensyEWMU: Format PCB BOM and add PDF version
</commit_message>
<xml_diff>
--- a/src/SimLinkup/HardwareSupport/TeensyEWMU/PCB/BOM_PCB rev 1_01 2021-05-24.XLSX
+++ b/src/SimLinkup/HardwareSupport/TeensyEWMU/PCB/BOM_PCB rev 1_01 2021-05-24.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lightningstools\src\SimLinkup\HardwareSupport\TeensyEWMU\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AEC9E0-6FCF-42D7-9699-733FDFE40A90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3888986-797E-4F01-8912-9E25007CEA03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,7 +258,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +389,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -735,7 +741,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -748,7 +754,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -796,7 +806,121 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -807,6 +931,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{05CC2378-25E1-4A43-A8A0-1243A5C6CC5C}" name="Table1" displayName="Table1" ref="A1:G20" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:G20" xr:uid="{FD210E09-9BEB-4B08-95A8-F49F64D8D98D}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F9CD4C2C-2CF4-4379-9860-802248374C1D}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{AEBA19FE-1052-4683-8CAC-752740CF5CDC}" name="Designator"/>
+    <tableColumn id="3" xr3:uid="{B03EF1AA-25AF-49D8-80CF-1B1EBF872CEE}" name="Quantity"/>
+    <tableColumn id="4" xr3:uid="{BD1CB6A2-6A3D-4D3F-A6FF-EC5D8E7FE904}" name="Manufacturer Part" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{B5FFD496-8FB8-43A5-A549-0BD11FB0BF83}" name="Manufacturer" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{17088A8E-1377-4459-AD0F-B2AA5E9439C5}" name="Supplier" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{07268105-6C8E-49A7-9B28-8B542A1C940C}" name="Supplier Part" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1109,17 +1249,17 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
     <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" customWidth="1"/>
     <col min="4" max="4" width="18.796875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.9296875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1156,16 +1296,16 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1179,16 +1319,16 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1196,7 +1336,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4">
@@ -1219,7 +1359,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5">
@@ -1248,16 +1388,16 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1271,16 +1411,16 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1294,16 +1434,16 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1317,16 +1457,16 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1340,16 +1480,16 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>15244449</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1363,16 +1503,16 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="F11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1386,16 +1526,16 @@
       <c r="C12">
         <v>8</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="F12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1409,16 +1549,16 @@
       <c r="C13">
         <v>5</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1432,16 +1572,16 @@
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1455,16 +1595,16 @@
       <c r="C15">
         <v>5</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1478,16 +1618,16 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1501,16 +1641,16 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <v>61400416121</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1524,16 +1664,16 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="F18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1547,16 +1687,16 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="F19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1570,21 +1710,24 @@
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="F20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>